<commit_message>
json file change and OS Module
</commit_message>
<xml_diff>
--- a/Deepesh/PythonProgramming/PythonFileHandling/excel_files_operation/test_data.xlsx
+++ b/Deepesh/PythonProgramming/PythonFileHandling/excel_files_operation/test_data.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -394,8 +395,8 @@
   </sheetPr>
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -468,6 +469,17 @@
       <c r="B2" t="n">
         <v>4</v>
       </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>5*1</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -478,6 +490,17 @@
       <c r="B3" t="n">
         <v>5</v>
       </c>
+      <c r="D3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>5*2</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -488,6 +511,17 @@
       <c r="B4" t="n">
         <v>6</v>
       </c>
+      <c r="D4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>5*3</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -498,6 +532,17 @@
       <c r="B5" t="n">
         <v>7</v>
       </c>
+      <c r="D5" t="n">
+        <v>8</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>5*4</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -508,6 +553,17 @@
       <c r="B6" t="n">
         <v>8</v>
       </c>
+      <c r="D6" t="n">
+        <v>10</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>5*5</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -518,6 +574,17 @@
       <c r="B7" t="n">
         <v>9</v>
       </c>
+      <c r="D7" t="n">
+        <v>12</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>5*6</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -528,6 +595,17 @@
       <c r="B8" t="n">
         <v>10</v>
       </c>
+      <c r="D8" t="n">
+        <v>14</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>5*7</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -538,6 +616,17 @@
       <c r="B9" t="n">
         <v>11</v>
       </c>
+      <c r="D9" t="n">
+        <v>16</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>5*8</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -548,12 +637,34 @@
       <c r="B10" t="n">
         <v>12</v>
       </c>
+      <c r="D10" t="n">
+        <v>18</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>5*9</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
           <t>Bangalore</t>
         </is>
+      </c>
+      <c r="D11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>5*10</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="12">
@@ -819,4 +930,153 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>5*1</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>5*2</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>10</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>5*3</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C3" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>5*4</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>20</v>
+      </c>
+      <c r="C4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>5*5</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>25</v>
+      </c>
+      <c r="C5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5*6</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C6" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>5*7</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>35</v>
+      </c>
+      <c r="C7" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>5*8</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>40</v>
+      </c>
+      <c r="C8" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>5*9</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>45</v>
+      </c>
+      <c r="C9" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>5*10</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>50</v>
+      </c>
+      <c r="C10" t="n">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>